<commit_message>
Задача 2, fix test + testsuite - 22.07 v9
</commit_message>
<xml_diff>
--- a/Test_suite.xlsx
+++ b/Test_suite.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="98">
   <si>
     <t>ID</t>
   </si>
@@ -51,7 +51,7 @@
 Доступ к API.</t>
   </si>
   <si>
-    <t>1. Отправить POST запрос /wp/v2/posts на создание поста с параметрами slug, title, content, status</t>
+    <t>1. Отправить POST запрос /wp/v2/c на создание поста с параметрами slug, title, content, status</t>
   </si>
   <si>
     <t>1. Запрос API отправляется на сервер.</t>
@@ -296,7 +296,7 @@
     <t>DELETE - Отправка запроса удаления пользователя</t>
   </si>
   <si>
-    <t>1. Отправить DELETE запрос /wp/v2/users/&lt;id&gt; для удаления объекта</t>
+    <t>1. Отправить DELETE запрос /wp/v2/users/&lt;id&gt; для удаления объекта с параметрами reassign и force:</t>
   </si>
   <si>
     <t>3. Тело ответа в формате JSON объекта &lt;id&gt; с измененным параметром  "deleted" в статусе "true":
@@ -449,6 +449,42 @@
   </si>
   <si>
     <t>4. В базе данных у комментария &lt;id&gt; в параметре "comment_approved" статус "trash"</t>
+  </si>
+  <si>
+    <t>Создание в бд и тест через API</t>
+  </si>
+  <si>
+    <t>создать тест кейсы на проверку получения данных через api запрос</t>
+  </si>
+  <si>
+    <t>READ USER - Отправка запроса чтения данных пользователя</t>
+  </si>
+  <si>
+    <t>Создано тестовое окружение с Wordpress и БД к нему.
+Активирован плагин JSON Basic Authentification.
+Доступ к API.
+Доступ к базовой авторизации.
+В базе данных создан пользователь с обязательными полями</t>
+  </si>
+  <si>
+    <t>READ POST - Отправка запроса чтения созданного поста</t>
+  </si>
+  <si>
+    <t>Создано тестовое окружение с Wordpress и БД к нему.
+Активирован плагин JSON Basic Authentification.
+Доступ к API.
+В базе данных создан пост с параметрами slug, title, content, status.</t>
+  </si>
+  <si>
+    <t>READ COMMENT - Отправка запроса чтения созданного комментария</t>
+  </si>
+  <si>
+    <t>Создано тестовое окружение с Wordpress и БД к нему.
+Активирован плагин JSON Basic Authentification.
+Доступ к API.
+Базовая авторизация.
+В базе данных создан пост с возможностью комментирования (параметр "comment_status" в статусе "open")  и параметрами slug, title, content, status, author.
+В базе данных создан комментарий с параметрами post, content, author.</t>
   </si>
 </sst>
 </file>
@@ -591,7 +627,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="39">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -692,16 +728,13 @@
     <xf borderId="9" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="9" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="9" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="9" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1872,63 +1905,220 @@
       <c r="H52" s="34"/>
     </row>
     <row r="53">
-      <c r="A53" s="36"/>
-      <c r="B53" s="36"/>
-      <c r="C53" s="37"/>
-      <c r="D53" s="37"/>
-      <c r="E53" s="38"/>
-      <c r="F53" s="38"/>
-      <c r="G53" s="38"/>
+      <c r="A53" s="4"/>
+      <c r="B53" s="4"/>
+      <c r="C53" s="4"/>
+      <c r="D53" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="E53" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="F53" s="4"/>
+      <c r="G53" s="6"/>
+      <c r="H53" s="4"/>
     </row>
     <row r="54">
-      <c r="A54" s="3"/>
-      <c r="B54" s="3"/>
+      <c r="A54" s="7">
+        <v>6.0</v>
+      </c>
+      <c r="B54" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C54" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="D54" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="E54" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="F54" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="G54" s="11"/>
+      <c r="H54" s="12" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="55">
-      <c r="A55" s="3"/>
-      <c r="B55" s="3"/>
+      <c r="A55" s="14"/>
+      <c r="B55" s="15"/>
+      <c r="C55" s="16"/>
+      <c r="D55" s="17"/>
+      <c r="E55" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="F55" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="G55" s="11"/>
+      <c r="H55" s="18"/>
     </row>
     <row r="56">
-      <c r="A56" s="3"/>
-      <c r="B56" s="3"/>
+      <c r="A56" s="27"/>
+      <c r="B56" s="14"/>
+      <c r="C56" s="28"/>
+      <c r="D56" s="17"/>
+      <c r="E56" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="F56" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="G56" s="11"/>
+      <c r="H56" s="21"/>
     </row>
     <row r="57">
-      <c r="A57" s="3"/>
-      <c r="B57" s="3"/>
+      <c r="A57" s="29"/>
+      <c r="B57" s="30"/>
+      <c r="C57" s="28"/>
+      <c r="D57" s="17"/>
+      <c r="E57" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="F57" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="G57" s="11"/>
+      <c r="H57" s="21"/>
     </row>
     <row r="58">
-      <c r="A58" s="3"/>
-      <c r="B58" s="3"/>
+      <c r="A58" s="7">
+        <v>2.0</v>
+      </c>
+      <c r="B58" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C58" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="D58" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="E58" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F58" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="G58" s="11"/>
+      <c r="H58" s="12" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="59">
-      <c r="A59" s="3"/>
-      <c r="B59" s="3"/>
+      <c r="A59" s="14"/>
+      <c r="B59" s="15"/>
+      <c r="C59" s="16"/>
+      <c r="D59" s="17"/>
+      <c r="E59" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="F59" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="G59" s="11"/>
+      <c r="H59" s="18"/>
     </row>
     <row r="60">
-      <c r="A60" s="3"/>
-      <c r="B60" s="3"/>
-      <c r="C60" s="39"/>
+      <c r="A60" s="14"/>
+      <c r="B60" s="19"/>
+      <c r="C60" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="D60" s="17"/>
+      <c r="E60" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="F60" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="G60" s="11"/>
+      <c r="H60" s="18"/>
     </row>
     <row r="61">
-      <c r="A61" s="3"/>
-      <c r="B61" s="3"/>
-      <c r="C61" s="39"/>
+      <c r="A61" s="14"/>
+      <c r="B61" s="19"/>
+      <c r="C61" s="16"/>
+      <c r="D61" s="17"/>
+      <c r="E61" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="F61" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="G61" s="11"/>
+      <c r="H61" s="18"/>
     </row>
     <row r="62">
-      <c r="A62" s="3"/>
-      <c r="B62" s="3"/>
+      <c r="A62" s="7">
+        <v>10.0</v>
+      </c>
+      <c r="B62" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C62" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="D62" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="E62" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="F62" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="G62" s="11"/>
+      <c r="H62" s="12" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="63">
-      <c r="A63" s="3"/>
-      <c r="B63" s="3"/>
+      <c r="A63" s="14"/>
+      <c r="B63" s="15"/>
+      <c r="C63" s="16"/>
+      <c r="D63" s="17"/>
+      <c r="E63" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="F63" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="G63" s="11"/>
+      <c r="H63" s="18"/>
     </row>
     <row r="64">
-      <c r="A64" s="3"/>
-      <c r="B64" s="3"/>
+      <c r="A64" s="14"/>
+      <c r="B64" s="19"/>
+      <c r="C64" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="D64" s="17"/>
+      <c r="E64" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="F64" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="G64" s="11"/>
+      <c r="H64" s="18"/>
     </row>
     <row r="65">
-      <c r="A65" s="3"/>
-      <c r="B65" s="3"/>
+      <c r="A65" s="30"/>
+      <c r="B65" s="36"/>
+      <c r="C65" s="37"/>
+      <c r="D65" s="33"/>
+      <c r="E65" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="F65" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="G65" s="11"/>
+      <c r="H65" s="38"/>
     </row>
     <row r="66">
       <c r="A66" s="3"/>
@@ -5742,39 +5932,26 @@
       <c r="A1018" s="3"/>
       <c r="B1018" s="3"/>
     </row>
-    <row r="1019">
-      <c r="A1019" s="3"/>
-      <c r="B1019" s="3"/>
-    </row>
-    <row r="1020">
-      <c r="A1020" s="3"/>
-      <c r="B1020" s="3"/>
-    </row>
-    <row r="1021">
-      <c r="A1021" s="3"/>
-      <c r="B1021" s="3"/>
-    </row>
-    <row r="1022">
-      <c r="A1022" s="3"/>
-      <c r="B1022" s="3"/>
-    </row>
   </sheetData>
-  <mergeCells count="12">
-    <mergeCell ref="D37:D40"/>
-    <mergeCell ref="D45:D48"/>
-    <mergeCell ref="D49:D52"/>
-    <mergeCell ref="D32:D35"/>
-    <mergeCell ref="D41:D44"/>
+  <mergeCells count="15">
     <mergeCell ref="D3:D6"/>
     <mergeCell ref="D7:D10"/>
     <mergeCell ref="D11:D14"/>
     <mergeCell ref="D15:D18"/>
-    <mergeCell ref="D28:D31"/>
     <mergeCell ref="D20:D23"/>
     <mergeCell ref="D24:D27"/>
+    <mergeCell ref="D28:D31"/>
+    <mergeCell ref="D32:D35"/>
+    <mergeCell ref="D37:D40"/>
+    <mergeCell ref="D41:D44"/>
+    <mergeCell ref="D45:D48"/>
+    <mergeCell ref="D49:D52"/>
+    <mergeCell ref="D54:D57"/>
+    <mergeCell ref="D58:D61"/>
+    <mergeCell ref="D62:D65"/>
   </mergeCells>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G3:G18 G20:G35 G37:G52">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="G3:G18 G20:G35 G37:G52 G54:G65">
       <formula1>"Passed ,Failed,Blocked"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Задача 2, testsuite - 22.07 v9
</commit_message>
<xml_diff>
--- a/Test_suite.xlsx
+++ b/Test_suite.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="97">
   <si>
     <t>ID</t>
   </si>
@@ -451,10 +451,7 @@
     <t>4. В базе данных у комментария &lt;id&gt; в параметре "comment_approved" статус "trash"</t>
   </si>
   <si>
-    <t>Создание в бд и тест через API</t>
-  </si>
-  <si>
-    <t>создать тест кейсы на проверку получения данных через api запрос</t>
+    <t>Создание данных в БД и тест API</t>
   </si>
   <si>
     <t>READ USER - Отправка запроса чтения данных пользователя</t>
@@ -1911,9 +1908,7 @@
       <c r="D53" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="E53" s="5" t="s">
-        <v>91</v>
-      </c>
+      <c r="E53" s="5"/>
       <c r="F53" s="4"/>
       <c r="G53" s="6"/>
       <c r="H53" s="4"/>
@@ -1926,10 +1921,10 @@
         <v>9</v>
       </c>
       <c r="C54" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="D54" s="9" t="s">
         <v>92</v>
-      </c>
-      <c r="D54" s="9" t="s">
-        <v>93</v>
       </c>
       <c r="E54" s="10" t="s">
         <v>53</v>
@@ -1992,10 +1987,10 @@
         <v>9</v>
       </c>
       <c r="C58" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="D58" s="9" t="s">
         <v>94</v>
-      </c>
-      <c r="D58" s="9" t="s">
-        <v>95</v>
       </c>
       <c r="E58" s="10" t="s">
         <v>24</v>
@@ -2060,10 +2055,10 @@
         <v>9</v>
       </c>
       <c r="C62" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="D62" s="9" t="s">
         <v>96</v>
-      </c>
-      <c r="D62" s="9" t="s">
-        <v>97</v>
       </c>
       <c r="E62" s="10" t="s">
         <v>76</v>

</xml_diff>